<commit_message>
Fixed a issue in notebook
</commit_message>
<xml_diff>
--- a/conversion.xlsx
+++ b/conversion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\Remapping Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CF3604-8655-4F86-8B4F-B7545618E3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC5F545-B71E-44D9-9F47-34D07CA7A78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4695" yWindow="3600" windowWidth="30930" windowHeight="15435" xr2:uid="{1E709FDD-82E7-4D18-BDFE-969612B1B9EE}"/>
+    <workbookView xWindow="4695" yWindow="3600" windowWidth="30930" windowHeight="15435" activeTab="1" xr2:uid="{1E709FDD-82E7-4D18-BDFE-969612B1B9EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Explanation" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="82">
   <si>
     <t>New_Variable</t>
   </si>
@@ -102,12 +102,6 @@
     <t>A_UNIT</t>
   </si>
   <si>
-    <t>Normal5#a</t>
-  </si>
-  <si>
-    <t>Normal5_Unit#a</t>
-  </si>
-  <si>
     <t>Normal6</t>
   </si>
   <si>
@@ -189,18 +183,9 @@
     <t>Converts keys based on Key_Table</t>
   </si>
   <si>
-    <t>Replaces column header, when empty no remapping, when filled remapping; e.g. 1 -&gt; a</t>
-  </si>
-  <si>
     <t>Adds a unit (e.g. 'Celcius') when Map_Variable (=New_Variable) is not empty</t>
   </si>
   <si>
-    <t>Converts a checkbox mapping to an option, e.g. NormalA#1 -&gt; Normal3 with value 'a'</t>
-  </si>
-  <si>
-    <t>Converts an option to a checkbox mapping; eg NormalC=1 -&gt; Normal5#a = 1</t>
-  </si>
-  <si>
     <t>**</t>
   </si>
   <si>
@@ -265,6 +250,39 @@
   </si>
   <si>
     <t>Do not place the Excels with mapping &amp; configuration data in a different folder</t>
+  </si>
+  <si>
+    <t>{"option1":"a", "option2":"b"}</t>
+  </si>
+  <si>
+    <t>{"1":"option1", "2":"option2"}</t>
+  </si>
+  <si>
+    <t>Normal5_Unit#option1</t>
+  </si>
+  <si>
+    <t>Normal5#option1</t>
+  </si>
+  <si>
+    <t>MeasureUnit</t>
+  </si>
+  <si>
+    <t>Replaces column header, when empty no remapping, when filled remapping; e.g. option1 -&gt; a</t>
+  </si>
+  <si>
+    <t>Converts a checkbox mapping to an option, e.g. NormalA#option1 -&gt; Normal3 with value 'a'</t>
+  </si>
+  <si>
+    <t>Converts an option to a checkbox mapping; eg NormalC=1 -&gt; Normal5#option1 = 1</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>{"option1":"1", "option2":"2"}</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
@@ -386,7 +404,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -396,6 +414,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="3"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -403,7 +423,22 @@
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="11">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -466,7 +501,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9AE4542F-9F68-485E-BBE8-B9FEA9E3DC09}" name="Table15" displayName="Table15" ref="A2:D15" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9AE4542F-9F68-485E-BBE8-B9FEA9E3DC09}" name="Table15" displayName="Table15" ref="A2:D15" totalsRowShown="0" headerRowDxfId="10">
   <autoFilter ref="A2:D15" xr:uid="{383FDB88-F083-4CDF-B03D-AFE7141D47C4}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{F3CBDC26-DCC0-4BFD-8D06-40CD89F11564}" name="New_Variable"/>
@@ -490,24 +525,24 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{383FDB88-F083-4CDF-B03D-AFE7141D47C4}" name="Table1" displayName="Table1" ref="A1:D14" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{383FDB88-F083-4CDF-B03D-AFE7141D47C4}" name="Table1" displayName="Table1" ref="A1:D14" totalsRowShown="0" headerRowDxfId="9" dataDxfId="0">
   <autoFilter ref="A1:D14" xr:uid="{383FDB88-F083-4CDF-B03D-AFE7141D47C4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E142AF83-5691-4FFC-9325-BE0C7B6FEAEA}" name="New_Variable"/>
-    <tableColumn id="2" xr3:uid="{E2732F87-DBC8-4585-9AD9-9E2C28FCE04F}" name="TypeOfConversion"/>
-    <tableColumn id="3" xr3:uid="{9C0642D5-E8C4-48C0-ABA0-1F6F938B5350}" name="Map_Variable"/>
-    <tableColumn id="4" xr3:uid="{CFDB804E-AB86-49C8-8388-E8DAAE906ACB}" name="Conversion"/>
+    <tableColumn id="1" xr3:uid="{E142AF83-5691-4FFC-9325-BE0C7B6FEAEA}" name="New_Variable" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{E2732F87-DBC8-4585-9AD9-9E2C28FCE04F}" name="TypeOfConversion" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{9C0642D5-E8C4-48C0-ABA0-1F6F938B5350}" name="Map_Variable" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{CFDB804E-AB86-49C8-8388-E8DAAE906ACB}" name="Conversion" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{60E7149A-D671-4822-9274-9F55ED5DFB04}" name="Table2" displayName="Table2" ref="A1:B5" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{60E7149A-D671-4822-9274-9F55ED5DFB04}" name="Table2" displayName="Table2" ref="A1:B5" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:B5" xr:uid="{60E7149A-D671-4822-9274-9F55ED5DFB04}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{1CDD68C5-C487-4D8D-B4B0-EEB954AB12DC}" name="Key_New" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{1353201A-7382-4450-A3A7-A64B29216D2B}" name="Key_Old" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{1CDD68C5-C487-4D8D-B4B0-EEB954AB12DC}" name="Key_New" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{1353201A-7382-4450-A3A7-A64B29216D2B}" name="Key_Old" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -823,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB16E3F3-6009-44A7-8F83-4CBF6605F01E}">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,7 +873,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -860,20 +895,20 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
         <v>29</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s">
-        <v>31</v>
       </c>
       <c r="D3" s="1"/>
       <c r="G3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -893,7 +928,7 @@
         <v>2</v>
       </c>
       <c r="H4" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -913,7 +948,7 @@
         <v>17</v>
       </c>
       <c r="H5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -927,13 +962,13 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="G6" t="s">
         <v>11</v>
       </c>
       <c r="H6" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -972,55 +1007,58 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="G9" t="s">
         <v>12</v>
       </c>
       <c r="H9" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>73</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" t="s">
-        <v>13</v>
+        <v>74</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
@@ -1031,16 +1069,16 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -1051,19 +1089,19 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
         <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D14">
         <v>4</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -1074,7 +1112,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
@@ -1085,12 +1123,12 @@
     </row>
     <row r="18" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
         <v>14</v>
@@ -1098,85 +1136,85 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G20" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G21" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G22" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G23" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G24" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G25" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B29" s="7"/>
       <c r="G29" s="7" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
@@ -1186,10 +1224,10 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G30" s="8" t="s">
         <v>67</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>72</v>
       </c>
       <c r="H30" s="8"/>
       <c r="I30" s="8"/>
@@ -1199,10 +1237,10 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G31" s="8" t="s">
         <v>68</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>73</v>
       </c>
       <c r="H31" s="8"/>
       <c r="I31" s="8"/>
@@ -1212,7 +1250,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G32" s="8" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
@@ -1222,7 +1260,7 @@
     </row>
     <row r="33" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G33" s="8" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
@@ -1232,7 +1270,7 @@
     </row>
     <row r="34" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G34" s="8" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
@@ -1259,16 +1297,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{760AE619-E443-4395-BB8D-172BD6E93BCC}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1286,172 +1324,176 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="9"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
-        <v>10</v>
+      <c r="D5" s="3" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D8" t="s">
-        <v>10</v>
+      <c r="D8" s="3" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D11" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>13</v>
-      </c>
+      <c r="D14" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -1484,10 +1526,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1500,7 +1542,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -1508,7 +1550,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -1516,7 +1558,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
@@ -1547,7 +1589,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
         <v>14</v>
@@ -1555,50 +1597,50 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed the issue in conversions.py as well, added comments in both
</commit_message>
<xml_diff>
--- a/conversion.xlsx
+++ b/conversion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\Remapping Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC5F545-B71E-44D9-9F47-34D07CA7A78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0C9ACD-7B82-451E-BB41-7F6254D7EFE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4695" yWindow="3600" windowWidth="30930" windowHeight="15435" activeTab="1" xr2:uid="{1E709FDD-82E7-4D18-BDFE-969612B1B9EE}"/>
+    <workbookView xWindow="76680" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{1E709FDD-82E7-4D18-BDFE-969612B1B9EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Explanation" sheetId="5" r:id="rId1"/>
@@ -525,24 +525,24 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{383FDB88-F083-4CDF-B03D-AFE7141D47C4}" name="Table1" displayName="Table1" ref="A1:D14" totalsRowShown="0" headerRowDxfId="9" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{383FDB88-F083-4CDF-B03D-AFE7141D47C4}" name="Table1" displayName="Table1" ref="A1:D14" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A1:D14" xr:uid="{383FDB88-F083-4CDF-B03D-AFE7141D47C4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E142AF83-5691-4FFC-9325-BE0C7B6FEAEA}" name="New_Variable" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{E2732F87-DBC8-4585-9AD9-9E2C28FCE04F}" name="TypeOfConversion" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{9C0642D5-E8C4-48C0-ABA0-1F6F938B5350}" name="Map_Variable" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{CFDB804E-AB86-49C8-8388-E8DAAE906ACB}" name="Conversion" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{E142AF83-5691-4FFC-9325-BE0C7B6FEAEA}" name="New_Variable" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{E2732F87-DBC8-4585-9AD9-9E2C28FCE04F}" name="TypeOfConversion" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{9C0642D5-E8C4-48C0-ABA0-1F6F938B5350}" name="Map_Variable" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{CFDB804E-AB86-49C8-8388-E8DAAE906ACB}" name="Conversion" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{60E7149A-D671-4822-9274-9F55ED5DFB04}" name="Table2" displayName="Table2" ref="A1:B5" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{60E7149A-D671-4822-9274-9F55ED5DFB04}" name="Table2" displayName="Table2" ref="A1:B5" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="A1:B5" xr:uid="{60E7149A-D671-4822-9274-9F55ED5DFB04}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{1CDD68C5-C487-4D8D-B4B0-EEB954AB12DC}" name="Key_New" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{1353201A-7382-4450-A3A7-A64B29216D2B}" name="Key_Old" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{1CDD68C5-C487-4D8D-B4B0-EEB954AB12DC}" name="Key_New" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{1353201A-7382-4450-A3A7-A64B29216D2B}" name="Key_Old" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -858,7 +858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB16E3F3-6009-44A7-8F83-4CBF6605F01E}">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -867,7 +867,7 @@
     <col min="1" max="1" width="23.140625" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" customWidth="1"/>
     <col min="7" max="7" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1297,8 +1297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{760AE619-E443-4395-BB8D-172BD6E93BCC}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1514,9 +1514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52FACC24-7102-4663-A563-97415C02CCA1}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1577,8 +1575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{647F3D03-9604-45FA-805B-B7EE8B0FC232}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Bug fix and new conversion option SWAP
</commit_message>
<xml_diff>
--- a/conversion.xlsx
+++ b/conversion.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DAB81E8-CA16-4100-856F-513A9D8AEBD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="76920" yWindow="8340" windowWidth="24285" windowHeight="12360" activeTab="1" xr2:uid="{1E709FDD-82E7-4D18-BDFE-969612B1B9EE}"/>
+    <workbookView activeTab="0" windowHeight="12360" windowWidth="24285" xWindow="76920" xr2:uid="{1E709FDD-82E7-4D18-BDFE-969612B1B9EE}" yWindow="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Explanation" sheetId="5" r:id="rId1"/>
@@ -287,72 +287,125 @@
   <si>
     <t>1</t>
   </si>
+  <si>
+    <t>Normal,Unit,Check2Option,Option2Check,ID</t>
+  </si>
+  <si>
+    <t>Normal,Unit,Check2Option,Option2Check,ID</t>
+  </si>
+  <si>
+    <t>temp_A</t>
+  </si>
+  <si>
+    <t>temp_B</t>
+  </si>
+  <si>
+    <t>A_set</t>
+  </si>
+  <si>
+    <t>B_set</t>
+  </si>
+  <si>
+    <t>tem_B</t>
+  </si>
+  <si>
+    <t>Swap</t>
+  </si>
+  <si>
+    <t>Normal,Unit,Check2Option,Option2Check,ID</t>
+  </si>
+  <si>
+    <t>Normal,Unit,Check2Option,Option2Check,ID</t>
+  </si>
+  <si>
+    <t>Swam</t>
+  </si>
+  <si>
+    <t>Swamps the sets, A_set -&gt; B_set &amp; B_set to A_set</t>
+  </si>
+  <si>
+    <t>Don forget to add this one, other wise it would be in the output</t>
+  </si>
+  <si>
+    <t>**Don't forget to add this line, otherwise B_set won't appear in the output</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" count="8" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="8">
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);(&quot;$&quot;#,##0)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red](&quot;$&quot;#,##0)"/>
+    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);(&quot;$&quot;#,##0.00)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red](&quot;$&quot;#,##0.00)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* (#,##0);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* (#,##0);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* (#,##0.00);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* (#,##0.00);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="8">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF006100"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF9C5700"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b/>
+      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="8"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b/>
+      <color rgb="FF000000"/>
+      <sz val="16"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF9C0006"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -371,7 +424,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FF4472C4"/>
         <bgColor theme="4"/>
       </patternFill>
     </fill>
@@ -380,44 +433,66 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC00"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color rgb="FF8EAADB"/>
       </top>
       <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color rgb="FF8EAADB"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
   </borders>
   <cellStyleXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -857,23 +932,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB16E3F3-6009-44A7-8F83-4CBF6605F01E}">
-  <dimension ref="A1:M34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB16E3F3-6009-44A7-8F83-4CBF6605F01E}">
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScale="160" workbookViewId="0" zoomScaleNormal="160">
+      <selection pane="topLeft" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.140625" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" customWidth="1"/>
     <col min="4" max="4" width="29.28515625" customWidth="1"/>
     <col min="7" max="7" width="24.140625" customWidth="1"/>
+    <col min="8" max="8" width="8.26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row ht="21" r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>52</v>
       </c>
@@ -1123,136 +1198,151 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A18" s="6" t="s">
+    <row r="16">
+      <c r="A16" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+    </row>
+    <row ht="21" r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" t="s">
-        <v>35</v>
-      </c>
-      <c r="G20" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
-      </c>
-      <c r="G21" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G24" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B25" t="s">
         <v>40</v>
       </c>
       <c r="G25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A28" s="6" t="s">
+    <row ht="21" r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A30" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G28" s="6" t="s">
+      <c r="G30" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B29" s="7"/>
-      <c r="G29" s="7" t="s">
+      <c r="B31" s="7"/>
+      <c r="G31" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G30" s="8" t="s">
+      <c r="G32" s="8" t="s">
         <v>67</v>
-      </c>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G32" s="8" t="s">
-        <v>66</v>
       </c>
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
@@ -1260,9 +1350,12 @@
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>
     </row>
-    <row r="33" spans="7:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="G33" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
@@ -1270,9 +1363,9 @@
       <c r="K33" s="8"/>
       <c r="L33" s="8"/>
     </row>
-    <row r="34" spans="7:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G34" s="8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
@@ -1280,9 +1373,29 @@
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
     </row>
+    <row r="35" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G35" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+    </row>
+    <row r="36" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G36" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B15" xr:uid="{C0DAA8EB-A05D-4FF1-90A8-3BB14737FE62}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B15">
       <formula1>"Normal,Unit,Check2Option,Option2Check,ID"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1296,14 +1409,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{760AE619-E443-4395-BB8D-172BD6E93BCC}">
-  <dimension ref="A1:D14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{760AE619-E443-4395-BB8D-172BD6E93BCC}">
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView zoomScale="205" workbookViewId="0" tabSelected="1" zoomScaleNormal="205">
+      <selection pane="topLeft" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.5703125" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
@@ -1494,10 +1606,32 @@
         <v>13</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B6 B9" xr:uid="{08149D67-390C-443A-BC50-BCCC1473A6EE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B6 B9">
       <formula1>"Normal,Unit,Check2Option,Option2Check,ID"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1510,14 +1644,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52FACC24-7102-4663-A563-97415C02CCA1}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52FACC24-7102-4663-A563-97415C02CCA1}">
   <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B5"/>
+    <sheetView zoomScale="205" workbookViewId="0" zoomScaleNormal="205">
+      <selection pane="topLeft" activeCell="A2" sqref="A2:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.5703125" style="3" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" style="3" customWidth="1"/>
@@ -1573,14 +1706,13 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{647F3D03-9604-45FA-805B-B7EE8B0FC232}">
-  <dimension ref="A1:B7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{647F3D03-9604-45FA-805B-B7EE8B0FC232}">
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B7"/>
+    <sheetView zoomScale="175" workbookViewId="0" zoomScaleNormal="175">
+      <selection pane="topLeft" activeCell="B2" sqref="B2:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>

</xml_diff>

<commit_message>
Adding date conversion to ISO 8601
</commit_message>
<xml_diff>
--- a/conversion.xlsx
+++ b/conversion.xlsx
@@ -328,6 +328,30 @@
   </si>
   <si>
     <t>**Don't forget to add this line, otherwise B_set won't appear in the output</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>D-M-Y</t>
+  </si>
+  <si>
+    <t>%D-%M-%Y</t>
+  </si>
+  <si>
+    <t>%D/%M/%Y</t>
+  </si>
+  <si>
+    <t>%D/%m/%Y</t>
+  </si>
+  <si>
+    <t>%d/%m/%Y</t>
+  </si>
+  <si>
+    <t>Converts the format in column D into ISO 8601 (%Y-%m-%d)</t>
+  </si>
+  <si>
+    <t>Converts the format in column D into ISO 8601 (%Y-%m-%d), errors will be coded in the output to: "ERR: original value"</t>
   </si>
 </sst>
 </file>
@@ -935,7 +959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB16E3F3-6009-44A7-8F83-4CBF6605F01E}">
   <sheetViews>
     <sheetView zoomScale="160" workbookViewId="0" zoomScaleNormal="160">
-      <selection pane="topLeft" activeCell="I17" sqref="I17"/>
+      <selection pane="topLeft" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1235,6 +1259,26 @@
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row ht="21" r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
@@ -1412,7 +1456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{760AE619-E443-4395-BB8D-172BD6E93BCC}">
   <sheetViews>
     <sheetView zoomScale="205" workbookViewId="0" tabSelected="1" zoomScaleNormal="205">
-      <selection pane="topLeft" activeCell="A15" sqref="A15"/>
+      <selection pane="topLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1626,6 +1670,20 @@
       </c>
       <c r="C16" s="0" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding duration mapping based on two valid ISO8601 formated date variables
</commit_message>
<xml_diff>
--- a/conversion.xlsx
+++ b/conversion.xlsx
@@ -352,6 +352,33 @@
   </si>
   <si>
     <t>Converts the format in column D into ISO 8601 (%Y-%m-%d), errors will be coded in the output to: "ERR: original value"</t>
+  </si>
+  <si>
+    <t>Start_Date</t>
+  </si>
+  <si>
+    <t>End_Date</t>
+  </si>
+  <si>
+    <t>%Y-%m-%d</t>
+  </si>
+  <si>
+    <t>A_dur</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>{"Start_Date": "End_Date"}</t>
+  </si>
+  <si>
+    <t>End_date</t>
+  </si>
+  <si>
+    <t>%d-%m-%Y</t>
+  </si>
+  <si>
+    <t>End_Date - Start_Date in days, requires ISO 8601 formats, ERR when no valid duration</t>
   </si>
 </sst>
 </file>
@@ -429,7 +456,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -461,6 +488,9 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC00"/>
       </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid"/>
     </fill>
   </fills>
   <borders count="2">
@@ -505,7 +535,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -517,6 +547,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -959,7 +990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB16E3F3-6009-44A7-8F83-4CBF6605F01E}">
   <sheetViews>
     <sheetView zoomScale="160" workbookViewId="0" zoomScaleNormal="160">
-      <selection pane="topLeft" activeCell="H19" sqref="H19"/>
+      <selection pane="topLeft" activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1005,7 +1036,7 @@
         <v>29</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>28</v>
       </c>
       <c r="H3" t="s">
@@ -1025,7 +1056,7 @@
       <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H4" t="s">
@@ -1045,7 +1076,7 @@
       <c r="D5" t="s">
         <v>20</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H5" t="s">
@@ -1065,7 +1096,7 @@
       <c r="D6" t="s">
         <v>71</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H6" t="s">
@@ -1085,6 +1116,7 @@
       <c r="D7">
         <v>1</v>
       </c>
+      <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1096,6 +1128,7 @@
       <c r="C8" t="s">
         <v>6</v>
       </c>
+      <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1110,7 +1143,7 @@
       <c r="D9" t="s">
         <v>72</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H9" t="s">
@@ -1158,15 +1191,12 @@
       <c r="D12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1178,15 +1208,12 @@
       <c r="C13" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1201,15 +1228,12 @@
       <c r="D14">
         <v>4</v>
       </c>
-      <c r="G14" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1232,7 +1256,7 @@
       <c r="C16" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="G16" s="0" t="s">
+      <c r="G16" s="1" t="s">
         <v>90</v>
       </c>
       <c r="H16" s="0" t="s">
@@ -1249,6 +1273,7 @@
       <c r="C17" s="0" t="s">
         <v>88</v>
       </c>
+      <c r="G17" s="1"/>
       <c r="H17" s="5" t="s">
         <v>96</v>
       </c>
@@ -1262,180 +1287,248 @@
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>97</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="G18" s="0" t="s">
+      <c r="G18" s="1" t="s">
         <v>97</v>
       </c>
       <c r="H18" s="0" t="s">
         <v>104</v>
       </c>
     </row>
-    <row ht="21" r="20" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A20" s="6" t="s">
+    <row r="19">
+      <c r="A19" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="G22" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+    </row>
+    <row r="23">
+      <c r="G23" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+    </row>
+    <row r="24">
+      <c r="G24" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+    </row>
+    <row ht="21" r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" t="s">
-        <v>35</v>
-      </c>
-      <c r="G22" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" t="s">
-        <v>36</v>
-      </c>
-      <c r="G23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" t="s">
-        <v>38</v>
-      </c>
-      <c r="G24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" t="s">
-        <v>40</v>
-      </c>
-      <c r="G25" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
-      </c>
-      <c r="G26" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+      <c r="G27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" t="s">
+        <v>36</v>
+      </c>
+      <c r="G28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" t="s">
+        <v>38</v>
+      </c>
+      <c r="G29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" t="s">
+        <v>40</v>
+      </c>
+      <c r="G30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>43</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B32" t="s">
         <v>40</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G32" t="s">
         <v>59</v>
       </c>
     </row>
-    <row ht="21" r="30" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A30" s="6" t="s">
+    <row ht="21" r="35" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A35" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G30" s="6" t="s">
+      <c r="G35" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="7"/>
-      <c r="G31" s="7" t="s">
+      <c r="B36" s="7"/>
+      <c r="G36" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G32" s="8" t="s">
+      <c r="G37" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G33" s="8" t="s">
+      <c r="G38" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G34" s="8" t="s">
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G39" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
-    </row>
-    <row r="35" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G35" s="8" t="s">
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+    </row>
+    <row r="40" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G40" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-    </row>
-    <row r="36" spans="7:12" x14ac:dyDescent="0.25">
-      <c r="G36" s="8" t="s">
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
+    </row>
+    <row r="41" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G41" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="8"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -1456,7 +1549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{760AE619-E443-4395-BB8D-172BD6E93BCC}">
   <sheetViews>
     <sheetView zoomScale="205" workbookViewId="0" tabSelected="1" zoomScaleNormal="205">
-      <selection pane="topLeft" activeCell="D17" sqref="D17"/>
+      <selection pane="topLeft" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -1674,16 +1767,44 @@
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>97</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>102</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>